<commit_message>
NordVPN and Soundcloud make their entrance!
- Introduction of the NordVPN proxy switcher to collect data from platforms without API.

- Soundcloud statistics are now collected! The export method and the script to write weekly notes automatically have been modified accordingly.

- exe.py created to execute at once both data collection and report auto writting.

- Data for week 3 added. "Charts IN" and "All Time Data" updated.

+ minor changes
</commit_message>
<xml_diff>
--- a/2021 Charts IN.xlsx
+++ b/2021 Charts IN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylmp\Documents\[!] PROJETS PERSONNELS\[MUSIC] 2021 Charts\music_charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3893DB44-47D5-4E05-8A8D-F8763430F862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00611821-E9D9-459C-8F92-7D83C9B4EAE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="3195" windowWidth="21600" windowHeight="11835" xr2:uid="{54C79188-7736-4F11-96D1-FC3D6773F7C8}"/>
+    <workbookView xWindow="1200" yWindow="3735" windowWidth="21600" windowHeight="11835" xr2:uid="{54C79188-7736-4F11-96D1-FC3D6773F7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="294">
   <si>
     <t>Artist</t>
   </si>
@@ -162,9 +162,6 @@
     <t>History</t>
   </si>
   <si>
-    <t>Discover Records</t>
-  </si>
-  <si>
     <t>Future Bounce</t>
   </si>
   <si>
@@ -339,199 +336,577 @@
     <t>Melodic Dubstep</t>
   </si>
   <si>
+    <t>Julian Jordan</t>
+  </si>
+  <si>
+    <t>Big Bad Bass</t>
+  </si>
+  <si>
+    <t>upqk0sf</t>
+  </si>
+  <si>
+    <t>M91mEIF9He4</t>
+  </si>
+  <si>
+    <t>6zGu2XFS0Sg</t>
+  </si>
+  <si>
+    <t>atv4KA3qGEM</t>
+  </si>
+  <si>
+    <t>Jaxxwell</t>
+  </si>
+  <si>
+    <t>Castion</t>
+  </si>
+  <si>
+    <t>Banger Machine</t>
+  </si>
+  <si>
+    <t>Bass House</t>
+  </si>
+  <si>
+    <t>MI3t3PV9FRI</t>
+  </si>
+  <si>
+    <t>LAtRDn65gIg</t>
+  </si>
+  <si>
+    <t>124437h5</t>
+  </si>
+  <si>
+    <t>REGGIO, Rave Republic</t>
+  </si>
+  <si>
+    <t>Legacy</t>
+  </si>
+  <si>
+    <t>WbToys</t>
+  </si>
+  <si>
+    <t>Let Me Love You</t>
+  </si>
+  <si>
+    <t>HEXAGON, GenerationHEX</t>
+  </si>
+  <si>
+    <t>LX2Rv__tmeQ</t>
+  </si>
+  <si>
+    <t>QgtR4X8V-UA</t>
+  </si>
+  <si>
+    <t>41vcwWmMmyg</t>
+  </si>
+  <si>
+    <t>d3dGtDfjF1g</t>
+  </si>
+  <si>
+    <t>mxEMPOrxJRY</t>
+  </si>
+  <si>
+    <t>25jq92lx</t>
+  </si>
+  <si>
+    <t>deadmau5, Wolfgang Gartner</t>
+  </si>
+  <si>
+    <t>Channel 43</t>
+  </si>
+  <si>
+    <t>mau5trap</t>
+  </si>
+  <si>
+    <t>dy3QONktMoY</t>
+  </si>
+  <si>
+    <t>rC7WCKNzcag</t>
+  </si>
+  <si>
+    <t>LfCDDX9m5iU</t>
+  </si>
+  <si>
+    <t>1yzxx6dp</t>
+  </si>
+  <si>
+    <t>1rkpmdcf</t>
+  </si>
+  <si>
+    <t>1z010vv5</t>
+  </si>
+  <si>
+    <t>Track_Name</t>
+  </si>
+  <si>
+    <t>OlnxmYzJ7Oc</t>
+  </si>
+  <si>
+    <t>Misfit</t>
+  </si>
+  <si>
+    <t>Mirage</t>
+  </si>
+  <si>
+    <t>BreadnButter, Trap City</t>
+  </si>
+  <si>
+    <t>Trap</t>
+  </si>
+  <si>
+    <t>Firebomb</t>
+  </si>
+  <si>
+    <t>Hard Style</t>
+  </si>
+  <si>
+    <t>insaneintherainmusic</t>
+  </si>
+  <si>
+    <t>Bonetrousle</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>Dr Phunk, Diandra Faye</t>
+  </si>
+  <si>
+    <t>mf-gJutp0gE</t>
+  </si>
+  <si>
+    <t>I5EPbaJ3nvk</t>
+  </si>
+  <si>
+    <t>jtfbFgnzlww</t>
+  </si>
+  <si>
+    <t>M22AAALw7xA</t>
+  </si>
+  <si>
+    <t>L7J_5zE49Us</t>
+  </si>
+  <si>
+    <t>TpW3W8IN1hc</t>
+  </si>
+  <si>
+    <t>HoCHjUazAhI</t>
+  </si>
+  <si>
+    <t>2b5pkl8x</t>
+  </si>
+  <si>
+    <t>Bootshaus ID</t>
+  </si>
+  <si>
+    <t>RAMSSEY</t>
+  </si>
+  <si>
+    <t>Anubis</t>
+  </si>
+  <si>
+    <t>Tribal Trap</t>
+  </si>
+  <si>
+    <t>quoa6-myhAc</t>
+  </si>
+  <si>
+    <t>lr9FVXLMgmE</t>
+  </si>
+  <si>
+    <t>mURlTKt-F9s</t>
+  </si>
+  <si>
+    <t>2-JLb6AxrU8</t>
+  </si>
+  <si>
+    <t>Rezilient</t>
+  </si>
+  <si>
+    <t>Positive Reaction</t>
+  </si>
+  <si>
+    <t>Galacy, Liquicity</t>
+  </si>
+  <si>
+    <t>ik8fHRD1JkM</t>
+  </si>
+  <si>
+    <t>VHvwtNsXeyg</t>
+  </si>
+  <si>
+    <t>Kaskade</t>
+  </si>
+  <si>
+    <t>Closer</t>
+  </si>
+  <si>
+    <t>2MeX5PCp1LE</t>
+  </si>
+  <si>
+    <t>HcKNnaCpINI</t>
+  </si>
+  <si>
+    <t>Soundcloud_Link1</t>
+  </si>
+  <si>
+    <t>Soundcloud_Link2</t>
+  </si>
+  <si>
+    <t>jaxxwell-sc/bootshaus-id</t>
+  </si>
+  <si>
+    <t>liquicityrecords/polygon-coming-home-feat</t>
+  </si>
+  <si>
+    <t>polygonsound/polygon-coming-home-feat-martin-jasper</t>
+  </si>
+  <si>
+    <t>kiraramagic/wraith</t>
+  </si>
+  <si>
+    <t>jonthofficial/history</t>
+  </si>
+  <si>
+    <t>tribaltrapmusic/anubis</t>
+  </si>
+  <si>
+    <t>nocopyrightsounds/castion-banger-machine-ncs-release</t>
+  </si>
+  <si>
+    <t>dimmakrecords/slippy-free</t>
+  </si>
+  <si>
+    <t>simon-rosenfeld-official/dangerous-woman</t>
+  </si>
+  <si>
+    <t>nocopyrightsounds/arlow-shiah-maisel-21-ncs-release</t>
+  </si>
+  <si>
+    <t>aiobahn/moving-forward</t>
+  </si>
+  <si>
+    <t>hexagon/malarkey-shackles-radio-edit</t>
+  </si>
+  <si>
+    <t>deadmau5/deadmau5-wolfgang-gartner-channel-43-radio-edit</t>
+  </si>
+  <si>
+    <t>deadmau5/deadmau5-wolfgang-gartner-channel-43</t>
+  </si>
+  <si>
+    <t>hexagon/lulleaux-even-if-you-dont</t>
+  </si>
+  <si>
+    <t>future-house-cloud/losingcontrol</t>
+  </si>
+  <si>
+    <t>monstercat/tynan-ace-aura-stay</t>
+  </si>
+  <si>
+    <t>julianjordan/julian-jordan-big-bad-bass</t>
+  </si>
+  <si>
+    <t>hexagon/mo-falk-im-back</t>
+  </si>
+  <si>
+    <t>aspyermusic/symphony</t>
+  </si>
+  <si>
+    <t>revealed-recordings/reggio-rave-republic-legacy</t>
+  </si>
+  <si>
+    <t>hexagon/wbtoys-let-me-love-you</t>
+  </si>
+  <si>
+    <t>officialdrphunk/firebomb-feat-diandra-faye</t>
+  </si>
+  <si>
+    <t>brednbutterrec/misfit-mirage</t>
+  </si>
+  <si>
+    <t>liquicityrecords/rezilient-positive-reaction-1</t>
+  </si>
+  <si>
+    <t>ledgednb/rezilient-positive-reaction</t>
+  </si>
+  <si>
+    <t>monstercat/kaskade-closer</t>
+  </si>
+  <si>
+    <t>Discover Records, JompaMusic</t>
+  </si>
+  <si>
+    <t>M-f-r4HB7f0</t>
+  </si>
+  <si>
+    <t>NUZB</t>
+  </si>
+  <si>
+    <t>Nighttime</t>
+  </si>
+  <si>
+    <t>VEEkYEyS6-g</t>
+  </si>
+  <si>
+    <t>dLKLHi8BNH4</t>
+  </si>
+  <si>
+    <t>nuzb/nighttime</t>
+  </si>
+  <si>
+    <t>2d19up95</t>
+  </si>
+  <si>
+    <t>Saint Punk</t>
+  </si>
+  <si>
+    <t>Empty Bed</t>
+  </si>
+  <si>
+    <t>Maurice Lessing</t>
+  </si>
+  <si>
+    <t>Never Let You Go</t>
+  </si>
+  <si>
+    <t>dK2FJQX24Io</t>
+  </si>
+  <si>
+    <t>JyseEvj2nkE</t>
+  </si>
+  <si>
+    <t>PVkprgEY56w</t>
+  </si>
+  <si>
+    <t>DA-KI4Jjwzk</t>
+  </si>
+  <si>
+    <t>2fwxlcnx</t>
+  </si>
+  <si>
+    <t>1rkmk56x</t>
+  </si>
+  <si>
+    <t>monstercat/saint-punk-empty-bed</t>
+  </si>
+  <si>
+    <t>bv6x85p</t>
+  </si>
+  <si>
+    <t>hexagon/maurice-lessing-never-let-you-go</t>
+  </si>
+  <si>
+    <t>Lost World</t>
+  </si>
+  <si>
+    <t>Deekey</t>
+  </si>
+  <si>
+    <t>Without You</t>
+  </si>
+  <si>
+    <t>Revealed Recordings, Revealed Radar</t>
+  </si>
+  <si>
     <t>JLVQTenxaG8</t>
   </si>
   <si>
-    <t>Julian Jordan</t>
-  </si>
-  <si>
-    <t>Big Bad Bass</t>
-  </si>
-  <si>
-    <t>H9YRxnxktfU</t>
-  </si>
-  <si>
-    <t>PBHBXZcuWFE</t>
-  </si>
-  <si>
-    <t>HUUFGgzyyv8</t>
-  </si>
-  <si>
-    <t>upqk0sf</t>
-  </si>
-  <si>
-    <t>M91mEIF9He4</t>
-  </si>
-  <si>
-    <t>6zGu2XFS0Sg</t>
-  </si>
-  <si>
-    <t>atv4KA3qGEM</t>
-  </si>
-  <si>
-    <t>Jaxxwell</t>
-  </si>
-  <si>
-    <t>Castion</t>
-  </si>
-  <si>
-    <t>Banger Machine</t>
-  </si>
-  <si>
-    <t>Bass House</t>
-  </si>
-  <si>
-    <t>MI3t3PV9FRI</t>
-  </si>
-  <si>
-    <t>LAtRDn65gIg</t>
-  </si>
-  <si>
-    <t>124437h5</t>
-  </si>
-  <si>
-    <t>REGGIO, Rave Republic</t>
-  </si>
-  <si>
-    <t>Legacy</t>
-  </si>
-  <si>
-    <t>WbToys</t>
-  </si>
-  <si>
-    <t>Let Me Love You</t>
-  </si>
-  <si>
-    <t>HEXAGON, GenerationHEX</t>
-  </si>
-  <si>
-    <t>LX2Rv__tmeQ</t>
-  </si>
-  <si>
-    <t>QgtR4X8V-UA</t>
-  </si>
-  <si>
-    <t>41vcwWmMmyg</t>
-  </si>
-  <si>
-    <t>d3dGtDfjF1g</t>
-  </si>
-  <si>
-    <t>mxEMPOrxJRY</t>
-  </si>
-  <si>
-    <t>25jq92lx</t>
-  </si>
-  <si>
-    <t>deadmau5, Wolfgang Gartner</t>
-  </si>
-  <si>
-    <t>Channel 43</t>
-  </si>
-  <si>
-    <t>mau5trap</t>
-  </si>
-  <si>
-    <t>dy3QONktMoY</t>
-  </si>
-  <si>
-    <t>rC7WCKNzcag</t>
-  </si>
-  <si>
-    <t>LfCDDX9m5iU</t>
-  </si>
-  <si>
-    <t>1yzxx6dp</t>
-  </si>
-  <si>
-    <t>1rkpmdcf</t>
-  </si>
-  <si>
-    <t>1z010vv5</t>
-  </si>
-  <si>
-    <t>Track_Name</t>
-  </si>
-  <si>
-    <t>OlnxmYzJ7Oc</t>
-  </si>
-  <si>
-    <t>Misfit</t>
-  </si>
-  <si>
-    <t>Mirage</t>
-  </si>
-  <si>
-    <t>BreadnButter, Trap City</t>
-  </si>
-  <si>
-    <t>Trap</t>
-  </si>
-  <si>
-    <t>Firebomb</t>
-  </si>
-  <si>
-    <t>Hard Style</t>
-  </si>
-  <si>
-    <t>insaneintherainmusic</t>
-  </si>
-  <si>
-    <t>Bonetrousle</t>
-  </si>
-  <si>
-    <t>Jazz</t>
-  </si>
-  <si>
-    <t>Dr Phunk, Diandra Faye</t>
-  </si>
-  <si>
-    <t>mf-gJutp0gE</t>
-  </si>
-  <si>
-    <t>I5EPbaJ3nvk</t>
-  </si>
-  <si>
-    <t>jtfbFgnzlww</t>
-  </si>
-  <si>
-    <t>M22AAALw7xA</t>
-  </si>
-  <si>
-    <t>L7J_5zE49Us</t>
-  </si>
-  <si>
-    <t>TpW3W8IN1hc</t>
-  </si>
-  <si>
-    <t>HoCHjUazAhI</t>
-  </si>
-  <si>
-    <t>2b5pkl8x</t>
-  </si>
-  <si>
-    <t>Bootshaus ID</t>
-  </si>
-  <si>
-    <t>RAMSSEY</t>
-  </si>
-  <si>
-    <t>Anubis</t>
-  </si>
-  <si>
-    <t>Tribal Trap</t>
-  </si>
-  <si>
-    <t>quoa6-myhAc</t>
-  </si>
-  <si>
-    <t>lr9FVXLMgmE</t>
-  </si>
-  <si>
-    <t>mURlTKt-F9s</t>
-  </si>
-  <si>
-    <t>2-JLb6AxrU8</t>
+    <t>x-7fSAeWtwI</t>
+  </si>
+  <si>
+    <t>ibIT6WsB0L4</t>
+  </si>
+  <si>
+    <t>3zT91DPOI0w</t>
+  </si>
+  <si>
+    <t>2q91x77f</t>
+  </si>
+  <si>
+    <t>deekeymusic/without-you</t>
+  </si>
+  <si>
+    <t>deekeymusic/without-you-extended-mix</t>
+  </si>
+  <si>
+    <t>Feint</t>
+  </si>
+  <si>
+    <t>Do Better</t>
+  </si>
+  <si>
+    <t>Body Ocean</t>
+  </si>
+  <si>
+    <t>Once The Music</t>
+  </si>
+  <si>
+    <t>Tech House</t>
+  </si>
+  <si>
+    <t>Porter Robinson</t>
+  </si>
+  <si>
+    <t>Loot At The Sky</t>
+  </si>
+  <si>
+    <t>MOM+POP</t>
+  </si>
+  <si>
+    <t>D3EPANK</t>
+  </si>
+  <si>
+    <t>Eternally</t>
+  </si>
+  <si>
+    <t>MR.BLACK, Offer Nissim, Chester Young</t>
+  </si>
+  <si>
+    <t>Mucho Bien (Chester Young Remix)</t>
+  </si>
+  <si>
+    <t>Revealed Recordins</t>
+  </si>
+  <si>
+    <t>ticyjqmYptw</t>
+  </si>
+  <si>
+    <t>h_HKv1D_I-o</t>
+  </si>
+  <si>
+    <t>huJA0oBOBJg</t>
+  </si>
+  <si>
+    <t>WfOb61k6e_I</t>
+  </si>
+  <si>
+    <t>6g6VNLNyOsg</t>
+  </si>
+  <si>
+    <t>GKZNQCZHLGI</t>
+  </si>
+  <si>
+    <t>PuMz4v5PYKc</t>
+  </si>
+  <si>
+    <t>reaKcwuoz7o</t>
+  </si>
+  <si>
+    <t>Yu4YVcsQsQ8</t>
+  </si>
+  <si>
+    <t>iKAFo6GnEPw</t>
+  </si>
+  <si>
+    <t>XAQYXKxBexw</t>
+  </si>
+  <si>
+    <t>FCJybZ7bVkc</t>
+  </si>
+  <si>
+    <t>zrh5Lw9q9b4</t>
+  </si>
+  <si>
+    <t>2nfhu4gp</t>
+  </si>
+  <si>
+    <t>1uc4g77f</t>
+  </si>
+  <si>
+    <t>1dcysunp</t>
+  </si>
+  <si>
+    <t>lostidentitiesmusic/any-other-way-feat-anna-3</t>
+  </si>
+  <si>
+    <t>monstercat/feint-do-better</t>
+  </si>
+  <si>
+    <t>feintdnb/feint-do-better-master-v2</t>
+  </si>
+  <si>
+    <t>bodyocean/once-the-music</t>
+  </si>
+  <si>
+    <t>porter-robinson/look-at-the-sky</t>
+  </si>
+  <si>
+    <t>fhcselection/eternally</t>
+  </si>
+  <si>
+    <t>mrblackmusic/mucho-bien-chester-young-remix</t>
+  </si>
+  <si>
+    <t>Future House Cloud, FHC Selection</t>
+  </si>
+  <si>
+    <t>Lady Bee, Dame1</t>
+  </si>
+  <si>
+    <t>Mixmash Recorsds</t>
+  </si>
+  <si>
+    <t>Ghetto House</t>
+  </si>
+  <si>
+    <t>Bleu Clair, OOTORO</t>
+  </si>
+  <si>
+    <t>Beat Like This</t>
+  </si>
+  <si>
+    <t>FNoPSJl4qJI</t>
+  </si>
+  <si>
+    <t>Soon Not Later</t>
+  </si>
+  <si>
+    <t>IDHXaiih3Qs</t>
+  </si>
+  <si>
+    <t>ZoVgTP4KXcQ</t>
+  </si>
+  <si>
+    <t>hj8r1fp</t>
+  </si>
+  <si>
+    <t>ydzyvkf</t>
+  </si>
+  <si>
+    <t>mixmash-records/lady-bee-feat-dame1-soon-not-later</t>
+  </si>
+  <si>
+    <t>bleuclair/bleuclairbeatlikethis</t>
+  </si>
+  <si>
+    <t>DJ St3v3, Sebastian Mateo</t>
+  </si>
+  <si>
+    <t>So Sexy</t>
+  </si>
+  <si>
+    <t>WU38Zq1s2g0</t>
+  </si>
+  <si>
+    <t>6rthk7o0Qjs</t>
+  </si>
+  <si>
+    <t>InZ6eGW-hns</t>
+  </si>
+  <si>
+    <t>xldDLNQ_Y-8</t>
+  </si>
+  <si>
+    <t>13zt5ytf</t>
+  </si>
+  <si>
+    <t>sebastianmateomusic/so-sexy-extended-mix</t>
+  </si>
+  <si>
+    <t>sebastianmateomusic/so-sexy</t>
+  </si>
+  <si>
+    <t>sub71u5</t>
   </si>
 </sst>
 </file>
@@ -952,32 +1327,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE11BB-30C0-4383-BAC4-B91D2977671A}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="57.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="52.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -1001,15 +1378,21 @@
         <v>7</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -1029,38 +1412,48 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="E3" s="4">
         <v>44197</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1087,62 +1480,74 @@
         <v>15</v>
       </c>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E5" s="4">
         <v>44200</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E6" s="4">
         <v>44201</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1159,18 +1564,22 @@
         <v>44201</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1187,24 +1596,28 @@
         <v>44202</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -1213,16 +1626,20 @@
         <v>44203</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1239,81 +1656,95 @@
         <v>44203</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="4">
         <v>44203</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4">
         <v>44204</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>28</v>
@@ -1325,20 +1756,22 @@
         <v>44204</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -1355,18 +1788,22 @@
         <v>44204</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1374,10 +1811,10 @@
         <v>44</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E15" s="4">
         <v>44204</v>
@@ -1387,16 +1824,20 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>32</v>
@@ -1405,18 +1846,22 @@
         <v>44204</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -1431,16 +1876,18 @@
         <v>44205</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
@@ -1457,280 +1904,778 @@
         <v>44207</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>105</v>
+        <v>244</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4">
+        <v>44209</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="4">
-        <v>44210</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E20" s="4">
         <v>44210</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="J20" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E21" s="4">
         <v>44210</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>213</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="E22" s="4">
-        <v>44211</v>
+        <v>44210</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E23" s="4">
-        <v>44216</v>
+        <v>44210</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>127</v>
+        <v>78</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>125</v>
+        <v>223</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="4">
+        <v>44211</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="4">
-        <v>44216</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="E25" s="4">
-        <v>44522</v>
+        <v>44211</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>153</v>
+        <v>228</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>154</v>
+        <v>229</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>143</v>
+        <v>242</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>144</v>
+        <v>243</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>145</v>
+        <v>270</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="E26" s="4">
-        <v>44522</v>
+        <v>44216</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>157</v>
+        <v>256</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="4">
+        <v>44216</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="4">
+        <v>44216</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="4">
+        <v>44216</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="4">
+        <v>44217</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="4">
+        <v>44218</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="H31" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
+      <c r="I31" s="5"/>
+      <c r="J31" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" s="4">
+        <v>44218</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="4">
-        <v>44523</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="G32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="4">
+        <v>44218</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="4">
+        <v>44218</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="4">
+        <v>44219</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="4">
+        <v>44223</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="4">
+        <v>44223</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E38" s="4">
+        <v>44223</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E39" s="4">
+        <v>44225</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="4">
+        <v>44229</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" s="4">
+        <v>44231</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="L41" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J27">
-    <sortCondition ref="E2:E27"/>
-    <sortCondition ref="B2:B27"/>
-    <sortCondition ref="A2:A27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L41">
+    <sortCondition ref="E2:E41"/>
+    <sortCondition ref="B2:B41"/>
+    <sortCondition ref="A2:A41"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>